<commit_message>
Timeline has been updated
</commit_message>
<xml_diff>
--- a/Lhub_PT.xlsx
+++ b/Lhub_PT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Learning-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>ASSIGNED TO</t>
   </si>
@@ -152,6 +152,33 @@
       </rPr>
       <t>Lhub_PT_V1</t>
     </r>
+  </si>
+  <si>
+    <t>week 2</t>
+  </si>
+  <si>
+    <t>Design the Class Diagram</t>
+  </si>
+  <si>
+    <t>Farah</t>
+  </si>
+  <si>
+    <t>Nada</t>
+  </si>
+  <si>
+    <t>Design Peer Review Sheet</t>
+  </si>
+  <si>
+    <t>Design Data Flow Diagram(Lhub_DFD)</t>
+  </si>
+  <si>
+    <t>Design the Entity Relationship Diagram (ERD)(Lhub_ERD)</t>
+  </si>
+  <si>
+    <t>Design Use Case Diagrams(Lhub_usecase)</t>
+  </si>
+  <si>
+    <t>Design the Wireframes(Lhub_Wireframe)</t>
   </si>
 </sst>
 </file>
@@ -384,13 +411,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,7 +562,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$8:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>creating project plan doc (PP_DOC_1)</c:v>
                 </c:pt>
@@ -565,6 +592,24 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>project timeline (PT_DOC_10)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Design the Wireframes(Lhub_Wireframe)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Design Use Case Diagrams(Lhub_usecase)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Design the Entity Relationship Diagram (ERD)(Lhub_ERD)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Design the Class Diagram</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Design Data Flow Diagram(Lhub_DFD)</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Design Peer Review Sheet</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -604,6 +649,24 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>43582</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,7 +1020,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$8:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>creating project plan doc (PP_DOC_1)</c:v>
                 </c:pt>
@@ -987,6 +1050,24 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>project timeline (PT_DOC_10)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Design the Wireframes(Lhub_Wireframe)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Design Use Case Diagrams(Lhub_usecase)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Design the Entity Relationship Diagram (ERD)(Lhub_ERD)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Design the Class Diagram</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Design Data Flow Diagram(Lhub_DFD)</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Design Peer Review Sheet</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1025,6 +1106,24 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -1046,11 +1145,11 @@
         </c:dLbls>
         <c:gapWidth val="25"/>
         <c:overlap val="100"/>
-        <c:axId val="1018461168"/>
-        <c:axId val="1018470416"/>
+        <c:axId val="-1556538800"/>
+        <c:axId val="-1373949056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1018461168"/>
+        <c:axId val="-1556538800"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1093,7 +1192,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1018470416"/>
+        <c:crossAx val="-1373949056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1101,7 +1200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1018470416"/>
+        <c:axId val="-1373949056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="43582"/>
@@ -1153,7 +1252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1018461168"/>
+        <c:crossAx val="-1556538800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1774,7 +1873,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5937EF8B-69CA-AE46-8A64-0E3BA9BF5DCF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5937EF8B-69CA-AE46-8A64-0E3BA9BF5DCF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1810,7 +1909,7 @@
         <xdr:cNvPr id="6" name="Grafik 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F05858E-37C1-A94A-BA42-EFB31B87599F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F05858E-37C1-A94A-BA42-EFB31B87599F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1854,7 +1953,7 @@
         <xdr:cNvPr id="5" name="Grafik 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E67488F-1608-7941-8EFF-E1EF7E065CA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4E67488F-1608-7941-8EFF-E1EF7E065CA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2185,121 +2284,121 @@
   </sheetPr>
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="W15" sqref="W15"/>
+      <selection pane="topRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.3984375" customWidth="1"/>
-    <col min="2" max="2" width="18.69921875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" customWidth="1"/>
+    <col min="1" max="1" width="59.4140625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="11.19921875" customWidth="1"/>
-    <col min="6" max="6" width="9.796875" customWidth="1"/>
-    <col min="7" max="7" width="21.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
     </row>
-    <row r="2" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
     </row>
-    <row r="3" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
     </row>
-    <row r="4" spans="1:21" ht="147" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
+    <row r="4" spans="1:21" ht="147" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
     </row>
-    <row r="5" spans="1:21" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="147" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>28</v>
       </c>
@@ -2329,17 +2428,17 @@
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
     </row>
-    <row r="6" spans="1:21" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="147" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="24">
         <v>1</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <v>43587</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="23"/>
@@ -2360,7 +2459,7 @@
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
     </row>
-    <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2383,7 +2482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
@@ -2407,7 +2506,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
@@ -2421,7 +2520,7 @@
         <v>43589</v>
       </c>
       <c r="E9" s="14">
-        <f t="shared" ref="E9:E17" si="0">(D9-C9)</f>
+        <f t="shared" ref="E9:E23" si="0">(D9-C9)</f>
         <v>7</v>
       </c>
       <c r="F9" s="6">
@@ -2431,7 +2530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="18" t="s">
         <v>8</v>
       </c>
@@ -2455,7 +2554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
@@ -2479,7 +2578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="18" t="s">
         <v>10</v>
       </c>
@@ -2503,7 +2602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
@@ -2527,7 +2626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="18" t="s">
         <v>12</v>
       </c>
@@ -2551,7 +2650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="18" t="s">
         <v>13</v>
       </c>
@@ -2575,7 +2674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
@@ -2599,7 +2698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="19" t="s">
         <v>25</v>
       </c>
@@ -2623,61 +2722,151 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="8"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="12"/>
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="7">
+        <v>43589</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43596</v>
+      </c>
+      <c r="E18" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F18" s="6">
+        <v>100</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="8"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="12"/>
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7">
+        <v>43589</v>
+      </c>
+      <c r="D19" s="7">
+        <v>43596</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F19" s="6">
+        <v>100</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="8"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="12"/>
+    <row r="20" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="7">
+        <v>43589</v>
+      </c>
+      <c r="D20" s="7">
+        <v>43596</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F20" s="6">
+        <v>100</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="8"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="12"/>
+    <row r="21" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="7">
+        <v>43589</v>
+      </c>
+      <c r="D21" s="7">
+        <v>43596</v>
+      </c>
+      <c r="E21" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F21" s="6">
+        <v>100</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="8"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="13"/>
+    <row r="22" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="7">
+        <v>43589</v>
+      </c>
+      <c r="D22" s="7">
+        <v>43596</v>
+      </c>
+      <c r="E22" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F22" s="6">
+        <v>100</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="8"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="13"/>
+    <row r="23" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="7">
+        <v>43589</v>
+      </c>
+      <c r="D23" s="7">
+        <v>43596</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F23" s="6">
+        <v>100</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="24" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="8"/>
       <c r="B24" s="20"/>
       <c r="C24" s="7"/>
@@ -2686,7 +2875,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="21"/>
       <c r="C25" s="3"/>

</xml_diff>